<commit_message>
Update functions to generate graphs, and add them to the graphs folder
</commit_message>
<xml_diff>
--- a/graphs/Time to Pop from Stack.xlsx
+++ b/graphs/Time to Pop from Stack.xlsx
@@ -570,7 +570,7 @@
         <v>1000</v>
       </c>
       <c r="B1" t="n">
-        <v>2600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2">
@@ -578,7 +578,7 @@
         <v>2000</v>
       </c>
       <c r="B2" t="n">
-        <v>1400</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         <v>3000</v>
       </c>
       <c r="B3" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
@@ -594,7 +594,7 @@
         <v>4000</v>
       </c>
       <c r="B4" t="n">
-        <v>900</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5">
@@ -602,7 +602,7 @@
         <v>5000</v>
       </c>
       <c r="B5" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
         <v>6000</v>
       </c>
       <c r="B6" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7">
@@ -618,7 +618,7 @@
         <v>7000</v>
       </c>
       <c r="B7" t="n">
-        <v>800</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8">
@@ -626,7 +626,7 @@
         <v>8000</v>
       </c>
       <c r="B8" t="n">
-        <v>3600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
@@ -634,7 +634,7 @@
         <v>9000</v>
       </c>
       <c r="B9" t="n">
-        <v>1200</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10">
@@ -642,7 +642,7 @@
         <v>10000</v>
       </c>
       <c r="B10" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11">
@@ -650,7 +650,7 @@
         <v>11000</v>
       </c>
       <c r="B11" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12">
@@ -658,7 +658,7 @@
         <v>12000</v>
       </c>
       <c r="B12" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13">
@@ -666,7 +666,7 @@
         <v>13000</v>
       </c>
       <c r="B13" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14">
@@ -674,7 +674,7 @@
         <v>14000</v>
       </c>
       <c r="B14" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15">
@@ -682,7 +682,7 @@
         <v>15000</v>
       </c>
       <c r="B15" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16">
@@ -690,7 +690,7 @@
         <v>16000</v>
       </c>
       <c r="B16" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17">
@@ -698,7 +698,7 @@
         <v>17000</v>
       </c>
       <c r="B17" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="18">
@@ -706,7 +706,7 @@
         <v>18000</v>
       </c>
       <c r="B18" t="n">
-        <v>500</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="19">
@@ -714,7 +714,7 @@
         <v>19000</v>
       </c>
       <c r="B19" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20">
@@ -722,7 +722,7 @@
         <v>20000</v>
       </c>
       <c r="B20" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21">
@@ -730,7 +730,7 @@
         <v>21000</v>
       </c>
       <c r="B21" t="n">
-        <v>800</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22">
@@ -738,7 +738,7 @@
         <v>22000</v>
       </c>
       <c r="B22" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23">
@@ -746,7 +746,7 @@
         <v>23000</v>
       </c>
       <c r="B23" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24">
@@ -754,7 +754,7 @@
         <v>24000</v>
       </c>
       <c r="B24" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25">
@@ -762,7 +762,7 @@
         <v>25000</v>
       </c>
       <c r="B25" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26">
@@ -770,7 +770,7 @@
         <v>26000</v>
       </c>
       <c r="B26" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
@@ -778,7 +778,7 @@
         <v>27000</v>
       </c>
       <c r="B27" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28">
@@ -786,7 +786,7 @@
         <v>28000</v>
       </c>
       <c r="B28" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29">
@@ -794,7 +794,7 @@
         <v>29000</v>
       </c>
       <c r="B29" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30">
@@ -802,7 +802,7 @@
         <v>30000</v>
       </c>
       <c r="B30" t="n">
-        <v>600</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31">
@@ -810,7 +810,7 @@
         <v>31000</v>
       </c>
       <c r="B31" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32">
@@ -818,7 +818,7 @@
         <v>32000</v>
       </c>
       <c r="B32" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33">
@@ -826,7 +826,7 @@
         <v>33000</v>
       </c>
       <c r="B33" t="n">
-        <v>2000</v>
+        <v>700</v>
       </c>
     </row>
     <row r="34">
@@ -834,7 +834,7 @@
         <v>34000</v>
       </c>
       <c r="B34" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35">
@@ -842,7 +842,7 @@
         <v>35000</v>
       </c>
       <c r="B35" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36">
@@ -850,7 +850,7 @@
         <v>36000</v>
       </c>
       <c r="B36" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37">
@@ -858,7 +858,7 @@
         <v>37000</v>
       </c>
       <c r="B37" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38">
@@ -866,7 +866,7 @@
         <v>38000</v>
       </c>
       <c r="B38" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39">
@@ -874,7 +874,7 @@
         <v>39000</v>
       </c>
       <c r="B39" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40">
@@ -882,7 +882,7 @@
         <v>40000</v>
       </c>
       <c r="B40" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41">
@@ -890,7 +890,7 @@
         <v>41000</v>
       </c>
       <c r="B41" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42">
@@ -898,7 +898,7 @@
         <v>42000</v>
       </c>
       <c r="B42" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43">
@@ -922,7 +922,7 @@
         <v>45000</v>
       </c>
       <c r="B45" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46">
@@ -930,7 +930,7 @@
         <v>46000</v>
       </c>
       <c r="B46" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47">
@@ -946,7 +946,7 @@
         <v>48000</v>
       </c>
       <c r="B48" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49">
@@ -954,7 +954,7 @@
         <v>49000</v>
       </c>
       <c r="B49" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50">
@@ -962,7 +962,7 @@
         <v>50000</v>
       </c>
       <c r="B50" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51">
@@ -970,7 +970,7 @@
         <v>51000</v>
       </c>
       <c r="B51" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52">
@@ -994,7 +994,7 @@
         <v>54000</v>
       </c>
       <c r="B54" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55">
@@ -1018,7 +1018,7 @@
         <v>57000</v>
       </c>
       <c r="B57" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58">
@@ -1026,7 +1026,7 @@
         <v>58000</v>
       </c>
       <c r="B58" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59">
@@ -1034,7 +1034,7 @@
         <v>59000</v>
       </c>
       <c r="B59" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60">
@@ -1042,7 +1042,7 @@
         <v>60000</v>
       </c>
       <c r="B60" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61">
@@ -1050,7 +1050,7 @@
         <v>61000</v>
       </c>
       <c r="B61" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62">
@@ -1066,7 +1066,7 @@
         <v>63000</v>
       </c>
       <c r="B63" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64">
@@ -1074,7 +1074,7 @@
         <v>64000</v>
       </c>
       <c r="B64" t="n">
-        <v>900</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         <v>65000</v>
       </c>
       <c r="B65" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="66">
@@ -1090,7 +1090,7 @@
         <v>66000</v>
       </c>
       <c r="B66" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67">
@@ -1098,7 +1098,7 @@
         <v>67000</v>
       </c>
       <c r="B67" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68">
@@ -1114,7 +1114,7 @@
         <v>69000</v>
       </c>
       <c r="B69" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70">
@@ -1122,7 +1122,7 @@
         <v>70000</v>
       </c>
       <c r="B70" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71">
@@ -1130,7 +1130,7 @@
         <v>71000</v>
       </c>
       <c r="B71" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72">
@@ -1146,7 +1146,7 @@
         <v>73000</v>
       </c>
       <c r="B73" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74">
@@ -1154,7 +1154,7 @@
         <v>74000</v>
       </c>
       <c r="B74" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="75">
@@ -1178,7 +1178,7 @@
         <v>77000</v>
       </c>
       <c r="B77" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78">
@@ -1186,7 +1186,7 @@
         <v>78000</v>
       </c>
       <c r="B78" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79">
@@ -1194,7 +1194,7 @@
         <v>79000</v>
       </c>
       <c r="B79" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80">
@@ -1202,7 +1202,7 @@
         <v>80000</v>
       </c>
       <c r="B80" t="n">
-        <v>700</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81">
@@ -1210,7 +1210,7 @@
         <v>81000</v>
       </c>
       <c r="B81" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82">
@@ -1218,7 +1218,7 @@
         <v>82000</v>
       </c>
       <c r="B82" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83">
@@ -1226,7 +1226,7 @@
         <v>83000</v>
       </c>
       <c r="B83" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84">
@@ -1234,7 +1234,7 @@
         <v>84000</v>
       </c>
       <c r="B84" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85">
@@ -1242,7 +1242,7 @@
         <v>85000</v>
       </c>
       <c r="B85" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86">
@@ -1250,7 +1250,7 @@
         <v>86000</v>
       </c>
       <c r="B86" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87">
@@ -1258,7 +1258,7 @@
         <v>87000</v>
       </c>
       <c r="B87" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88">
@@ -1266,7 +1266,7 @@
         <v>88000</v>
       </c>
       <c r="B88" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89">
@@ -1274,7 +1274,7 @@
         <v>89000</v>
       </c>
       <c r="B89" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90">
@@ -1290,7 +1290,7 @@
         <v>91000</v>
       </c>
       <c r="B91" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92">
@@ -1298,7 +1298,7 @@
         <v>92000</v>
       </c>
       <c r="B92" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93">
@@ -1306,7 +1306,7 @@
         <v>93000</v>
       </c>
       <c r="B93" t="n">
-        <v>5800</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94">
@@ -1330,7 +1330,7 @@
         <v>96000</v>
       </c>
       <c r="B96" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97">
@@ -1338,7 +1338,7 @@
         <v>97000</v>
       </c>
       <c r="B97" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98">
@@ -1346,7 +1346,7 @@
         <v>98000</v>
       </c>
       <c r="B98" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99">
@@ -1354,7 +1354,7 @@
         <v>99000</v>
       </c>
       <c r="B99" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100">
@@ -1362,7 +1362,7 @@
         <v>100000</v>
       </c>
       <c r="B100" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>